<commit_message>
update <test>: excel sheet minor updates
</commit_message>
<xml_diff>
--- a/Test Cases/Hacker Kermit - AC Control System.xlsx
+++ b/Test Cases/Hacker Kermit - AC Control System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Courses\Sprints\Automotive Software BootCamp\Part 07 - Embedded Systems L2\S_ESL2_CAP_PROJECT_01 Simple Air Conditioner\AC_Control_System\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB3AF2E-3766-4233-881A-4CA69554A58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8ED8F2-99AE-4C91-A59F-003DEFD8349F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Backlog" sheetId="1" r:id="rId1"/>
@@ -268,6 +268,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 1. Call DIO_portInit with valid parameters
  2. Call DIO_portWrite with a value of 0x55 and a mask of  </t>
@@ -278,6 +279,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>0xFF (DIO_NO_MASK)</t>
     </r>
@@ -286,6 +288,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  3. Call DIO_portToggle with a mask of  </t>
@@ -296,6 +299,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>0xFF (DIO_NO_MASK)</t>
     </r>
@@ -304,6 +308,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  4. Call DIO_portWrite with a value of 0xAA and a mask of  </t>
@@ -314,6 +319,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>0xFF (DIO_NO_MASK)</t>
     </r>
@@ -322,6 +328,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  5. Call DIO_portToggle with a mask of  </t>
@@ -332,6 +339,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>0xFF (DIO_NO_MASK)</t>
     </r>
@@ -613,6 +621,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Rows Pins are set as </t>
     </r>
@@ -622,6 +631,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Output</t>
     </r>
@@ -630,6 +640,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">, Columns Pins are set as </t>
     </r>
@@ -639,6 +650,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Input</t>
     </r>
@@ -647,6 +659,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (enabling pullup resistor)</t>
     </r>
@@ -666,6 +679,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Rows Pins are set as </t>
     </r>
@@ -675,6 +689,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Output</t>
     </r>
@@ -683,6 +698,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (enable or re-enable KPD)</t>
     </r>
@@ -702,6 +718,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Rows Pins are set as </t>
     </r>
@@ -711,6 +728,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Input</t>
     </r>
@@ -719,6 +737,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (disable KPD)</t>
     </r>
@@ -809,6 +828,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 0xFF (DIO_NO_MASK)</t>
     </r>
@@ -833,107 +853,126 @@
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1209,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1325,43 +1364,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1371,7 +1373,41 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1380,7 +1416,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1406,8 +1448,8 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>24921</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>344229</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3570</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2867025" cy="2867025"/>
     <xdr:pic>
@@ -1429,7 +1471,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9350629" y="690060"/>
+          <a:off x="9348215" y="684888"/>
           <a:ext cx="2867025" cy="2867025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1689,8 +1731,8 @@
   </sheetPr>
   <dimension ref="A1:H1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1705,16 +1747,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1732,29 +1776,27 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="65" t="s">
-        <v>203</v>
-      </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
     </row>
     <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1825,13 +1867,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1851,13 +1893,13 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -1878,28 +1920,28 @@
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="51"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="52"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="49"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1953,13 +1995,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="49"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -2030,13 +2072,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -2057,28 +2099,28 @@
     </row>
     <row r="26" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="51"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="52"/>
     </row>
     <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
     </row>
     <row r="28" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
     </row>
     <row r="29" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -2098,13 +2140,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
     </row>
     <row r="31" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -2141,13 +2183,13 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="49"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -2188,13 +2230,13 @@
       <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
     </row>
     <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
@@ -5141,12 +5183,7 @@
       <c r="E1009" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A33:E33"/>
+  <mergeCells count="17">
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A19:E19"/>
@@ -5155,11 +5192,15 @@
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F1:H2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5:C8 C10 C12 C16:C18 C20:C23 C25 C29 C31:C32 C34:C35 C38:C39" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5178,14 +5219,14 @@
   </sheetPr>
   <dimension ref="A1:Z1027"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
     <col min="3" max="3" width="62.109375" customWidth="1"/>
     <col min="4" max="4" width="53.88671875" customWidth="1"/>
     <col min="5" max="5" width="37.77734375" customWidth="1"/>
@@ -5195,15 +5236,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -5224,20 +5267,18 @@
       <c r="F2" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="68" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:26" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="60"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
@@ -5261,14 +5302,14 @@
       <c r="Z3" s="20"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
@@ -5317,7 +5358,7 @@
       <c r="B6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="46" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="23" t="s">
@@ -5357,7 +5398,7 @@
       <c r="B7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="46" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="23" t="s">
@@ -5397,7 +5438,7 @@
       <c r="B8" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="46" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="23" t="s">
@@ -5477,7 +5518,7 @@
       <c r="B10" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="46" t="s">
         <v>202</v>
       </c>
       <c r="D10" s="23" t="s">
@@ -5557,7 +5598,7 @@
       <c r="B12" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="45" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="23" t="s">
@@ -5571,14 +5612,14 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -5761,14 +5802,14 @@
       <c r="Z17" s="27"/>
     </row>
     <row r="18" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63"/>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
@@ -5917,7 +5958,7 @@
       <c r="B22" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="47" t="s">
         <v>113</v>
       </c>
       <c r="D22" s="33" t="s">
@@ -5994,10 +6035,10 @@
       <c r="A24" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="60"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -6021,14 +6062,14 @@
       <c r="Z24" s="20"/>
     </row>
     <row r="25" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="57"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="63"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
@@ -6171,14 +6212,14 @@
       <c r="Z28" s="20"/>
     </row>
     <row r="29" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="63"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
@@ -6407,7 +6448,7 @@
       <c r="B35" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="62" t="s">
+      <c r="C35" s="45" t="s">
         <v>150</v>
       </c>
       <c r="D35" s="23" t="s">
@@ -6481,14 +6522,14 @@
       <c r="Z36" s="20"/>
     </row>
     <row r="37" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="57"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="63"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
@@ -6517,10 +6558,10 @@
       <c r="B38" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="62" t="s">
+      <c r="C38" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="45" t="s">
         <v>160</v>
       </c>
       <c r="E38" s="24" t="s">
@@ -6557,10 +6598,10 @@
       <c r="B39" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="62" t="s">
+      <c r="C39" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D39" s="45" t="s">
         <v>164</v>
       </c>
       <c r="E39" s="24" t="s">
@@ -6591,14 +6632,14 @@
       <c r="Z39" s="20"/>
     </row>
     <row r="40" spans="1:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
@@ -6812,10 +6853,10 @@
       <c r="A46" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
       <c r="F46" s="60"/>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -34361,7 +34402,8 @@
       <c r="Z1027" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="G1:I2"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A46:F46"/>

</xml_diff>